<commit_message>
Update Envío de Semana de Pruebas_links.xlsx
</commit_message>
<xml_diff>
--- a/Envío de Semana de Pruebas_links.xlsx
+++ b/Envío de Semana de Pruebas_links.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA INTELLIGENCE Dropbox\Diseño DATA's\Reuniones Ventas Municipios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvcma\Dropbox\Diseño DATA's\Reuniones Ventas Municipios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D42F59E-F8A3-4093-91D1-B56ABA3D6D8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B13E4BF-5999-4EB0-A807-010F54B3AD26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{3B4A1676-2C76-4DAF-976E-5D2F3133D93F}"/>
+    <workbookView xWindow="25590" yWindow="1650" windowWidth="10485" windowHeight="7875" xr2:uid="{3B4A1676-2C76-4DAF-976E-5D2F3133D93F}"/>
   </bookViews>
   <sheets>
     <sheet name="PRUEBAS MUNI" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1535" uniqueCount="606">
   <si>
     <t xml:space="preserve">Municipio </t>
   </si>
@@ -1897,6 +1897,22 @@
   </si>
   <si>
     <t>Comuna2</t>
+  </si>
+  <si>
+    <t>Cristian Casas</t>
+  </si>
+  <si>
+    <t>ccasas@munisanfelipe.cl</t>
+  </si>
+  <si>
+    <t>Marco Romero</t>
+  </si>
+  <si>
+    <t>Adaminitrador Municipal</t>
+  </si>
+  <si>
+    <t>marco.romero@riohurtado.cl
+administradormunicipal@riohurtado.cl</t>
   </si>
 </sst>
 </file>
@@ -1983,7 +1999,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -2054,12 +2070,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2184,12 +2211,65 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="22">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -2635,33 +2715,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CDDD1CD4-F13F-495E-9044-082F1923E939}" name="Tabla1" displayName="Tabla1" ref="A2:P79" totalsRowShown="0" headerRowDxfId="17" tableBorderDxfId="16">
-  <autoFilter ref="A2:P79" xr:uid="{CDDD1CD4-F13F-495E-9044-082F1923E939}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CDDD1CD4-F13F-495E-9044-082F1923E939}" name="Tabla1" displayName="Tabla1" ref="A2:P81" totalsRowShown="0" headerRowDxfId="21" tableBorderDxfId="20">
+  <autoFilter ref="A2:P81" xr:uid="{CDDD1CD4-F13F-495E-9044-082F1923E939}"/>
   <tableColumns count="16">
-    <tableColumn id="15" xr3:uid="{D06BE984-433D-4BFF-A541-8E8B197E9004}" name="id" dataDxfId="15">
+    <tableColumn id="15" xr3:uid="{D06BE984-433D-4BFF-A541-8E8B197E9004}" name="id" dataDxfId="19">
       <calculatedColumnFormula>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{005D3212-3A40-4B58-98D7-D1292D518F2A}" name="Codcom" dataDxfId="14">
+    <tableColumn id="14" xr3:uid="{005D3212-3A40-4B58-98D7-D1292D518F2A}" name="Codcom" dataDxfId="18">
       <calculatedColumnFormula>+IFERROR(VLOOKUP(Tabla1[[#This Row],[Municipio ]],Localiza[],2,0),"Corregir")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{7C4811B9-553D-402C-8AAE-419885E9449F}" name="Comuna" dataDxfId="13">
+    <tableColumn id="13" xr3:uid="{7C4811B9-553D-402C-8AAE-419885E9449F}" name="Comuna" dataDxfId="17">
       <calculatedColumnFormula>+IFERROR(VLOOKUP(Tabla1[[#This Row],[Codcom]],Localiza[[Codcom]:[Comuna2]],4,0),"Corregir")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{0E7C9871-2703-4B7F-B017-8FC983E1B3BE}" name="Región" dataDxfId="12">
+    <tableColumn id="16" xr3:uid="{0E7C9871-2703-4B7F-B017-8FC983E1B3BE}" name="Región" dataDxfId="16">
       <calculatedColumnFormula>+IFERROR(VLOOKUP(Tabla1[[#This Row],[Codcom]],Localiza[[Codcom]:[Comuna2]],3,0),"Corregir")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{128420C0-17E6-4C77-B24A-031CE5058FD6}" name="N°" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{D6A770A8-386A-411B-9533-00C2C2FFE47D}" name="Municipio " dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{527105F4-F27B-4877-BC35-7F33614E577B}" name="Día de reunión" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{E6BA65C4-8DC3-41A5-9CE2-0D35C250677E}" name="Funcionario(a)" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{75EE2533-C4B1-4338-9483-CDAF8802F627}" name="Cargo" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{A5A2B6F6-24AC-4F79-95C5-1053CF4A49BC}" name="Correos " dataDxfId="6" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="10" xr3:uid="{0D98D44A-E831-4829-86E7-5361BA65F1B4}" name="password" dataDxfId="5" dataCellStyle="Hipervínculo"/>
-    <tableColumn id="7" xr3:uid="{167FBB81-B95F-49E7-8C96-69A2D9C0D2E8}" name="Día para enviar la prueba" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{D41D5D40-B772-45FB-B04C-3320A684E80C}" name="Dia de envío " dataDxfId="3"/>
-    <tableColumn id="8" xr3:uid="{DF8FBEED-1178-47D1-8440-07DFAD957AA8}" name="Estado del correo" dataDxfId="2"/>
-    <tableColumn id="9" xr3:uid="{5078CCB7-43F3-41D1-876F-BFA095105361}" name="Comentarios de envio de prueba" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{183FF823-44FB-46DC-9581-132C380026ED}" name="Envío de correo de seguimiento" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{128420C0-17E6-4C77-B24A-031CE5058FD6}" name="N°" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{D6A770A8-386A-411B-9533-00C2C2FFE47D}" name="Municipio " dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{527105F4-F27B-4877-BC35-7F33614E577B}" name="Día de reunión" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{E6BA65C4-8DC3-41A5-9CE2-0D35C250677E}" name="Funcionario(a)" dataDxfId="12"/>
+    <tableColumn id="5" xr3:uid="{75EE2533-C4B1-4338-9483-CDAF8802F627}" name="Cargo" dataDxfId="11"/>
+    <tableColumn id="6" xr3:uid="{A5A2B6F6-24AC-4F79-95C5-1053CF4A49BC}" name="Correos " dataDxfId="10" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="10" xr3:uid="{0D98D44A-E831-4829-86E7-5361BA65F1B4}" name="password" dataDxfId="9" dataCellStyle="Hipervínculo"/>
+    <tableColumn id="7" xr3:uid="{167FBB81-B95F-49E7-8C96-69A2D9C0D2E8}" name="Día para enviar la prueba" dataDxfId="8"/>
+    <tableColumn id="11" xr3:uid="{D41D5D40-B772-45FB-B04C-3320A684E80C}" name="Dia de envío " dataDxfId="7"/>
+    <tableColumn id="8" xr3:uid="{DF8FBEED-1178-47D1-8440-07DFAD957AA8}" name="Estado del correo" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{5078CCB7-43F3-41D1-876F-BFA095105361}" name="Comentarios de envio de prueba" dataDxfId="5"/>
+    <tableColumn id="12" xr3:uid="{183FF823-44FB-46DC-9581-132C380026ED}" name="Envío de correo de seguimiento" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2978,30 +3058,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB1F595A-CBC7-490E-8B21-967F9C21CEA8}">
-  <dimension ref="A2:P79"/>
+  <dimension ref="A2:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" topLeftCell="J79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N81" sqref="N81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.109375" customWidth="1"/>
-    <col min="3" max="4" width="11.21875" customWidth="1"/>
-    <col min="5" max="5" width="5.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.44140625" customWidth="1"/>
-    <col min="7" max="7" width="17.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.5546875" customWidth="1"/>
-    <col min="9" max="10" width="24.44140625" customWidth="1"/>
-    <col min="11" max="11" width="17.5546875" style="7" customWidth="1"/>
-    <col min="12" max="12" width="15.33203125" customWidth="1"/>
-    <col min="13" max="13" width="15.77734375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="28.33203125" customWidth="1"/>
-    <col min="16" max="16" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" customWidth="1"/>
+    <col min="3" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.42578125" customWidth="1"/>
+    <col min="7" max="7" width="17.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" customWidth="1"/>
+    <col min="9" max="10" width="24.42578125" customWidth="1"/>
+    <col min="11" max="11" width="17.5703125" style="7" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.28515625" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>599</v>
       </c>
@@ -3051,7 +3131,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>12301-1</v>
@@ -3101,7 +3181,7 @@
         <v>44579</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>12301-1</v>
@@ -3151,7 +3231,7 @@
         <v>44579</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>13103-2</v>
@@ -3203,7 +3283,7 @@
         <v>44579</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>13103-2</v>
@@ -3255,7 +3335,7 @@
         <v>44579</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>10201-3</v>
@@ -3307,7 +3387,7 @@
       </c>
       <c r="P7" s="22"/>
     </row>
-    <row r="8" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>15102-4</v>
@@ -3359,7 +3439,7 @@
         <v>44579</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>15102-4</v>
@@ -3411,7 +3491,7 @@
         <v>44579</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>Corregir-5</v>
@@ -3463,7 +3543,7 @@
         <v>44579</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>Corregir-5</v>
@@ -3515,7 +3595,7 @@
         <v>44579</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>11401-6</v>
@@ -3567,7 +3647,7 @@
         <v>44579</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>13503-7</v>
@@ -3619,7 +3699,7 @@
         <v>44579</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>1101-8</v>
@@ -3669,7 +3749,7 @@
       </c>
       <c r="P14" s="27"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="24" x14ac:dyDescent="0.25">
       <c r="A15" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>7408-9</v>
@@ -3721,7 +3801,7 @@
         <v>44579</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>13403-10</v>
@@ -3773,7 +3853,7 @@
         <v>44579</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>13403-10</v>
@@ -3825,7 +3905,7 @@
         <v>44579</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>7302-11</v>
@@ -3877,7 +3957,7 @@
         <v>44579</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>7103-12</v>
@@ -3927,7 +4007,7 @@
       <c r="O19" s="21"/>
       <c r="P19" s="22"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>8312-13</v>
@@ -3979,7 +4059,7 @@
         <v>44579</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>Corregir-14</v>
@@ -4031,7 +4111,7 @@
         <v>44579</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>6304-15</v>
@@ -4083,7 +4163,7 @@
         <v>44579</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>8101-16</v>
@@ -4133,7 +4213,7 @@
       <c r="O23" s="35"/>
       <c r="P23" s="21"/>
     </row>
-    <row r="24" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>7304-17</v>
@@ -4183,7 +4263,7 @@
       <c r="O24" s="35"/>
       <c r="P24" s="21"/>
     </row>
-    <row r="25" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>8302-18</v>
@@ -4231,7 +4311,7 @@
       <c r="O25" s="35"/>
       <c r="P25" s="21"/>
     </row>
-    <row r="26" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>8302-18</v>
@@ -4279,7 +4359,7 @@
       <c r="O26" s="35"/>
       <c r="P26" s="21"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>7303-19</v>
@@ -4329,7 +4409,7 @@
       <c r="O27" s="35"/>
       <c r="P27" s="21"/>
     </row>
-    <row r="28" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>8203-20</v>
@@ -4379,7 +4459,7 @@
       <c r="O28" s="35"/>
       <c r="P28" s="21"/>
     </row>
-    <row r="29" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="36" x14ac:dyDescent="0.25">
       <c r="A29" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>13121-20</v>
@@ -4429,7 +4509,7 @@
       <c r="O29" s="35"/>
       <c r="P29" s="21"/>
     </row>
-    <row r="30" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="36" x14ac:dyDescent="0.25">
       <c r="A30" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>13121-21</v>
@@ -4477,7 +4557,7 @@
       <c r="O30" s="35"/>
       <c r="P30" s="21"/>
     </row>
-    <row r="31" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>10103-22</v>
@@ -4529,7 +4609,7 @@
       </c>
       <c r="P31" s="21"/>
     </row>
-    <row r="32" spans="1:16" ht="24" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="24" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>3202-23</v>
@@ -4579,7 +4659,7 @@
       <c r="O32" s="35"/>
       <c r="P32" s="21"/>
     </row>
-    <row r="33" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>13110-24</v>
@@ -4629,7 +4709,7 @@
       <c r="O33" s="35"/>
       <c r="P33" s="21"/>
     </row>
-    <row r="34" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>13110-24</v>
@@ -4679,7 +4759,7 @@
       <c r="O34" s="35"/>
       <c r="P34" s="21"/>
     </row>
-    <row r="35" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>Corregir-25</v>
@@ -4729,7 +4809,7 @@
       <c r="O35" s="35"/>
       <c r="P35" s="21"/>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>Corregir-26</v>
@@ -4781,7 +4861,7 @@
       </c>
       <c r="P36" s="21"/>
     </row>
-    <row r="37" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>Corregir-27</v>
@@ -4831,7 +4911,7 @@
       <c r="O37" s="35"/>
       <c r="P37" s="21"/>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:16" ht="24" x14ac:dyDescent="0.25">
       <c r="A38" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>13603-28</v>
@@ -4881,7 +4961,7 @@
       <c r="O38" s="35"/>
       <c r="P38" s="21"/>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:16" ht="24" x14ac:dyDescent="0.25">
       <c r="A39" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>13603-29</v>
@@ -4931,7 +5011,7 @@
       <c r="O39" s="35"/>
       <c r="P39" s="21"/>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:16" ht="24" x14ac:dyDescent="0.25">
       <c r="A40" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>13120-30</v>
@@ -4981,7 +5061,7 @@
       <c r="O40" s="21"/>
       <c r="P40" s="22"/>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:16" ht="24" x14ac:dyDescent="0.25">
       <c r="A41" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>13120-30</v>
@@ -5033,7 +5113,7 @@
       </c>
       <c r="P41" s="22"/>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>6308-31</v>
@@ -5083,7 +5163,7 @@
       <c r="O42" s="35"/>
       <c r="P42" s="21"/>
     </row>
-    <row r="43" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>16205-32</v>
@@ -5133,7 +5213,7 @@
       <c r="O43" s="35"/>
       <c r="P43" s="21"/>
     </row>
-    <row r="44" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>14103-33</v>
@@ -5185,7 +5265,7 @@
       </c>
       <c r="P44" s="21"/>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>10104-34</v>
@@ -5235,7 +5315,7 @@
       <c r="O45" s="35"/>
       <c r="P45" s="21"/>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>10104-34</v>
@@ -5285,7 +5365,7 @@
       <c r="O46" s="35"/>
       <c r="P46" s="21"/>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>10104-34</v>
@@ -5335,7 +5415,7 @@
       <c r="O47" s="35"/>
       <c r="P47" s="21"/>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>5604-35</v>
@@ -5387,7 +5467,7 @@
       </c>
       <c r="P48" s="21"/>
     </row>
-    <row r="49" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>Corregir-36</v>
@@ -5437,7 +5517,7 @@
       </c>
       <c r="P49" s="21"/>
     </row>
-    <row r="50" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A50" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>8205-37</v>
@@ -5485,7 +5565,7 @@
       <c r="O50" s="35"/>
       <c r="P50" s="21"/>
     </row>
-    <row r="51" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A51" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>Corregir-38</v>
@@ -5533,7 +5613,7 @@
       <c r="O51" s="35"/>
       <c r="P51" s="21"/>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>9101-39</v>
@@ -5583,7 +5663,7 @@
       </c>
       <c r="P52" s="21"/>
     </row>
-    <row r="53" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>Corregir-40</v>
@@ -5631,7 +5711,7 @@
       <c r="O53" s="35"/>
       <c r="P53" s="21"/>
     </row>
-    <row r="54" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A54" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>Corregir-40</v>
@@ -5679,7 +5759,7 @@
       <c r="O54" s="35"/>
       <c r="P54" s="21"/>
     </row>
-    <row r="55" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>Corregir-40</v>
@@ -5727,7 +5807,7 @@
       <c r="O55" s="35"/>
       <c r="P55" s="21"/>
     </row>
-    <row r="56" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>16107-41</v>
@@ -5777,7 +5857,7 @@
       </c>
       <c r="P56" s="21"/>
     </row>
-    <row r="57" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>16107-41</v>
@@ -5825,7 +5905,7 @@
       <c r="O57" s="35"/>
       <c r="P57" s="21"/>
     </row>
-    <row r="58" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>13129-42</v>
@@ -5875,7 +5955,7 @@
       </c>
       <c r="P58" s="21"/>
     </row>
-    <row r="59" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A59" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>15101-43</v>
@@ -5923,7 +6003,7 @@
       <c r="O59" s="35"/>
       <c r="P59" s="21"/>
     </row>
-    <row r="60" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>10209-44</v>
@@ -5971,7 +6051,7 @@
       <c r="O60" s="35"/>
       <c r="P60" s="21"/>
     </row>
-    <row r="61" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A61" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>12102-45</v>
@@ -6021,7 +6101,7 @@
       <c r="O61" s="35"/>
       <c r="P61" s="21"/>
     </row>
-    <row r="62" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A62" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>12103-46</v>
@@ -6073,7 +6153,7 @@
       </c>
       <c r="P62" s="21"/>
     </row>
-    <row r="63" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A63" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>5302-47</v>
@@ -6123,7 +6203,7 @@
       </c>
       <c r="P63" s="21"/>
     </row>
-    <row r="64" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A64" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>5302-47</v>
@@ -6173,7 +6253,7 @@
       </c>
       <c r="P64" s="21"/>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A65" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>5302-47</v>
@@ -6223,7 +6303,7 @@
       </c>
       <c r="P65" s="21"/>
     </row>
-    <row r="66" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A66" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>5102-48</v>
@@ -6271,7 +6351,7 @@
       <c r="O66" s="35"/>
       <c r="P66" s="21"/>
     </row>
-    <row r="67" spans="1:16" ht="72" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A67" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>13126-49</v>
@@ -6323,7 +6403,7 @@
       </c>
       <c r="P67" s="21"/>
     </row>
-    <row r="68" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>10102-50</v>
@@ -6373,7 +6453,7 @@
       </c>
       <c r="P68" s="21"/>
     </row>
-    <row r="69" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>5304-51</v>
@@ -6419,7 +6499,7 @@
       <c r="O69" s="35"/>
       <c r="P69" s="21"/>
     </row>
-    <row r="70" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>16108-52</v>
@@ -6467,7 +6547,7 @@
       <c r="O70" s="35"/>
       <c r="P70" s="21"/>
     </row>
-    <row r="71" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="A71" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>5705-53</v>
@@ -6513,7 +6593,7 @@
       <c r="O71" s="35"/>
       <c r="P71" s="21"/>
     </row>
-    <row r="72" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A72" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>16104-54</v>
@@ -6559,7 +6639,7 @@
       <c r="O72" s="35"/>
       <c r="P72" s="21"/>
     </row>
-    <row r="73" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>13125-55</v>
@@ -6605,7 +6685,7 @@
       <c r="O73" s="35"/>
       <c r="P73" s="21"/>
     </row>
-    <row r="74" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>16304-56</v>
@@ -6651,7 +6731,7 @@
       <c r="O74" s="35"/>
       <c r="P74" s="21"/>
     </row>
-    <row r="75" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="A75" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>Corregir-57</v>
@@ -6697,7 +6777,7 @@
       <c r="O75" s="35"/>
       <c r="P75" s="21"/>
     </row>
-    <row r="76" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>Corregir-58</v>
@@ -6743,7 +6823,7 @@
       <c r="O76" s="35"/>
       <c r="P76" s="21"/>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>Corregir-58</v>
@@ -6789,7 +6869,7 @@
       <c r="O77" s="35"/>
       <c r="P77" s="21"/>
     </row>
-    <row r="78" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>6107-59</v>
@@ -6835,7 +6915,7 @@
       <c r="O78" s="35"/>
       <c r="P78" s="21"/>
     </row>
-    <row r="79" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A79" s="40" t="str">
         <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
         <v>16301-60</v>
@@ -6881,20 +6961,112 @@
       <c r="O79" s="35"/>
       <c r="P79" s="35"/>
     </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A80" s="42" t="str">
+        <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
+        <v>5701-61</v>
+      </c>
+      <c r="B80" s="43">
+        <f>+IFERROR(VLOOKUP(Tabla1[[#This Row],[Municipio ]],Localiza[],2,0),"Corregir")</f>
+        <v>5701</v>
+      </c>
+      <c r="C80" s="44" t="str">
+        <f>+IFERROR(VLOOKUP(Tabla1[[#This Row],[Codcom]],Localiza[[Codcom]:[Comuna2]],4,0),"Corregir")</f>
+        <v>San Felipe</v>
+      </c>
+      <c r="D80" s="45" t="str">
+        <f>+IFERROR(VLOOKUP(Tabla1[[#This Row],[Codcom]],Localiza[[Codcom]:[Comuna2]],3,0),"Corregir")</f>
+        <v>Valparaíso</v>
+      </c>
+      <c r="E80" s="31">
+        <v>61</v>
+      </c>
+      <c r="F80" s="46" t="s">
+        <v>354</v>
+      </c>
+      <c r="G80" s="11">
+        <v>44580</v>
+      </c>
+      <c r="H80" s="12" t="s">
+        <v>601</v>
+      </c>
+      <c r="I80" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J80" s="32" t="s">
+        <v>602</v>
+      </c>
+      <c r="K80" s="32"/>
+      <c r="L80" s="33">
+        <v>44585</v>
+      </c>
+      <c r="M80" s="33"/>
+      <c r="N80" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="O80" s="35"/>
+      <c r="P80" s="35"/>
+    </row>
+    <row r="81" spans="1:16" ht="60" x14ac:dyDescent="0.25">
+      <c r="A81" s="42" t="str">
+        <f>+IFERROR(Tabla1[[#This Row],[Codcom]]&amp;"-"&amp;Tabla1[[#This Row],[N°]],"Corregir")</f>
+        <v>6305-62</v>
+      </c>
+      <c r="B81" s="43">
+        <f>+IFERROR(VLOOKUP(Tabla1[[#This Row],[Municipio ]],Localiza[],2,0),"Corregir")</f>
+        <v>6305</v>
+      </c>
+      <c r="C81" s="44" t="str">
+        <f>+IFERROR(VLOOKUP(Tabla1[[#This Row],[Codcom]],Localiza[[Codcom]:[Comuna2]],4,0),"Corregir")</f>
+        <v>Nancagua</v>
+      </c>
+      <c r="D81" s="45" t="str">
+        <f>+IFERROR(VLOOKUP(Tabla1[[#This Row],[Codcom]],Localiza[[Codcom]:[Comuna2]],3,0),"Corregir")</f>
+        <v>O'Higgins</v>
+      </c>
+      <c r="E81" s="31">
+        <v>62</v>
+      </c>
+      <c r="F81" s="46" t="s">
+        <v>389</v>
+      </c>
+      <c r="G81" s="11">
+        <v>37275</v>
+      </c>
+      <c r="H81" s="12" t="s">
+        <v>603</v>
+      </c>
+      <c r="I81" s="12" t="s">
+        <v>604</v>
+      </c>
+      <c r="J81" s="32" t="s">
+        <v>605</v>
+      </c>
+      <c r="K81" s="32"/>
+      <c r="L81" s="33">
+        <v>44585</v>
+      </c>
+      <c r="M81" s="33"/>
+      <c r="N81" s="34" t="s">
+        <v>55</v>
+      </c>
+      <c r="O81" s="35"/>
+      <c r="P81" s="35"/>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="K1:K2 K80:K1048576 N2:N79">
-    <cfRule type="cellIs" dxfId="21" priority="2" operator="equal">
+  <conditionalFormatting sqref="K1:K2 K80:K1048576 N2:N81">
+    <cfRule type="cellIs" dxfId="25" priority="2" operator="equal">
       <formula>"Por Enviar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="3" operator="equal">
       <formula>"Enviado"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="4" operator="equal">
       <formula>"No enviado"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3:D79">
-    <cfRule type="cellIs" dxfId="18" priority="1" operator="equal">
+  <conditionalFormatting sqref="A3:D81">
+    <cfRule type="cellIs" dxfId="22" priority="1" operator="equal">
       <formula>"Corregir"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6959,11 +7131,12 @@
     <hyperlink ref="J76" r:id="rId58" xr:uid="{765D8731-AE57-450D-AA17-1939A8783443}"/>
     <hyperlink ref="J77" r:id="rId59" xr:uid="{197073D0-C7B3-4E20-8DD5-ED450AAB7AB6}"/>
     <hyperlink ref="J78" r:id="rId60" xr:uid="{CD90595D-553C-4036-B09B-E589EA974698}"/>
+    <hyperlink ref="J80" r:id="rId61" xr:uid="{91D5FDD6-3096-4D48-9E60-070B7081873C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId61"/>
+  <pageSetup orientation="portrait" r:id="rId62"/>
   <tableParts count="1">
-    <tablePart r:id="rId62"/>
+    <tablePart r:id="rId63"/>
   </tableParts>
 </worksheet>
 </file>
@@ -6973,20 +7146,20 @@
   <dimension ref="A4:E350"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A330" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H345" sqref="H345"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.88671875" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>289</v>
       </c>
@@ -7003,7 +7176,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>510</v>
       </c>
@@ -7020,7 +7193,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>350</v>
       </c>
@@ -7037,7 +7210,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>562</v>
       </c>
@@ -7054,7 +7227,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>448</v>
       </c>
@@ -7071,7 +7244,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>312</v>
       </c>
@@ -7088,7 +7261,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>291</v>
       </c>
@@ -7105,7 +7278,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>488</v>
       </c>
@@ -7122,7 +7295,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>317</v>
       </c>
@@ -7139,7 +7312,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>470</v>
       </c>
@@ -7156,7 +7329,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>520</v>
       </c>
@@ -7173,7 +7346,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>297</v>
       </c>
@@ -7190,7 +7363,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>90</v>
       </c>
@@ -7207,7 +7380,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>433</v>
       </c>
@@ -7224,7 +7397,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>210</v>
       </c>
@@ -7241,7 +7414,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>559</v>
       </c>
@@ -7258,7 +7431,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>585</v>
       </c>
@@ -7275,7 +7448,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>340</v>
       </c>
@@ -7292,7 +7465,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>519</v>
       </c>
@@ -7309,7 +7482,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>438</v>
       </c>
@@ -7326,7 +7499,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>301</v>
       </c>
@@ -7343,7 +7516,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>241</v>
       </c>
@@ -7360,7 +7533,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>308</v>
       </c>
@@ -7377,7 +7550,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>345</v>
       </c>
@@ -7394,7 +7567,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -7411,7 +7584,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>227</v>
       </c>
@@ -7428,7 +7601,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>39</v>
       </c>
@@ -7445,7 +7618,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>293</v>
       </c>
@@ -7462,7 +7635,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>322</v>
       </c>
@@ -7479,7 +7652,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>100</v>
       </c>
@@ -7496,7 +7669,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>450</v>
       </c>
@@ -7513,7 +7686,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>351</v>
       </c>
@@ -7530,7 +7703,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>235</v>
       </c>
@@ -7547,7 +7720,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -7564,7 +7737,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>355</v>
       </c>
@@ -7581,7 +7754,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>403</v>
       </c>
@@ -7598,7 +7771,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>527</v>
       </c>
@@ -7615,7 +7788,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>528</v>
       </c>
@@ -7632,7 +7805,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>503</v>
       </c>
@@ -7649,7 +7822,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>404</v>
       </c>
@@ -7666,7 +7839,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>310</v>
       </c>
@@ -7683,7 +7856,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>387</v>
       </c>
@@ -7700,7 +7873,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>422</v>
       </c>
@@ -7717,7 +7890,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -7734,7 +7907,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>584</v>
       </c>
@@ -7751,7 +7924,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>586</v>
       </c>
@@ -7768,7 +7941,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>388</v>
       </c>
@@ -7785,7 +7958,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>469</v>
       </c>
@@ -7802,7 +7975,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>489</v>
       </c>
@@ -7819,7 +7992,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>511</v>
       </c>
@@ -7836,7 +8009,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>591</v>
       </c>
@@ -7853,7 +8026,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>136</v>
       </c>
@@ -7870,7 +8043,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>513</v>
       </c>
@@ -7887,7 +8060,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>365</v>
       </c>
@@ -7904,7 +8077,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>592</v>
       </c>
@@ -7921,7 +8094,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>508</v>
       </c>
@@ -7938,7 +8111,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>596</v>
       </c>
@@ -7955,7 +8128,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>366</v>
       </c>
@@ -7972,7 +8145,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>414</v>
       </c>
@@ -7989,7 +8162,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>294</v>
       </c>
@@ -8006,7 +8179,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>555</v>
       </c>
@@ -8023,7 +8196,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>471</v>
       </c>
@@ -8040,7 +8213,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>367</v>
       </c>
@@ -8057,7 +8230,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>326</v>
       </c>
@@ -8074,7 +8247,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>82</v>
       </c>
@@ -8091,7 +8264,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>529</v>
       </c>
@@ -8108,7 +8281,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>331</v>
       </c>
@@ -8125,7 +8298,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>396</v>
       </c>
@@ -8142,7 +8315,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>434</v>
       </c>
@@ -8159,7 +8332,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>307</v>
       </c>
@@ -8176,7 +8349,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>315</v>
       </c>
@@ -8193,7 +8366,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>421</v>
       </c>
@@ -8210,7 +8383,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>571</v>
       </c>
@@ -8227,7 +8400,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>451</v>
       </c>
@@ -8244,7 +8417,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>472</v>
       </c>
@@ -8261,7 +8434,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>52</v>
       </c>
@@ -8278,7 +8451,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>490</v>
       </c>
@@ -8295,7 +8468,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>177</v>
       </c>
@@ -8312,7 +8485,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>452</v>
       </c>
@@ -8329,7 +8502,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>15</v>
       </c>
@@ -8346,7 +8519,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>406</v>
       </c>
@@ -8363,7 +8536,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>491</v>
       </c>
@@ -8380,7 +8553,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>104</v>
       </c>
@@ -8397,7 +8570,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>368</v>
       </c>
@@ -8414,7 +8587,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>530</v>
       </c>
@@ -8431,7 +8604,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>256</v>
       </c>
@@ -8448,7 +8621,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>566</v>
       </c>
@@ -8465,7 +8638,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>169</v>
       </c>
@@ -8482,7 +8655,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>352</v>
       </c>
@@ -8499,7 +8672,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>397</v>
       </c>
@@ -8516,7 +8689,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>473</v>
       </c>
@@ -8533,7 +8706,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>531</v>
       </c>
@@ -8550,7 +8723,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>423</v>
       </c>
@@ -8567,7 +8740,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>453</v>
       </c>
@@ -8584,7 +8757,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>313</v>
       </c>
@@ -8601,7 +8774,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>159</v>
       </c>
@@ -8618,7 +8791,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>483</v>
       </c>
@@ -8635,7 +8808,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>504</v>
       </c>
@@ -8652,7 +8825,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>577</v>
       </c>
@@ -8669,7 +8842,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>454</v>
       </c>
@@ -8686,7 +8859,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>582</v>
       </c>
@@ -8703,7 +8876,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>455</v>
       </c>
@@ -8720,7 +8893,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>369</v>
       </c>
@@ -8737,7 +8910,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>512</v>
       </c>
@@ -8754,7 +8927,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>346</v>
       </c>
@@ -8771,7 +8944,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>505</v>
       </c>
@@ -8788,7 +8961,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>12</v>
       </c>
@@ -8805,7 +8978,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>431</v>
       </c>
@@ -8822,7 +8995,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>424</v>
       </c>
@@ -8839,7 +9012,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>295</v>
       </c>
@@ -8856,7 +9029,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>314</v>
       </c>
@@ -8873,7 +9046,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>532</v>
       </c>
@@ -8890,7 +9063,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>321</v>
       </c>
@@ -8907,7 +9080,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>533</v>
       </c>
@@ -8924,7 +9097,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>54</v>
       </c>
@@ -8941,7 +9114,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>125</v>
       </c>
@@ -8958,7 +9131,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>336</v>
       </c>
@@ -8975,7 +9148,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>332</v>
       </c>
@@ -8992,7 +9165,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>534</v>
       </c>
@@ -9009,7 +9182,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>347</v>
       </c>
@@ -9026,7 +9199,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>381</v>
       </c>
@@ -9043,7 +9216,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>108</v>
       </c>
@@ -9060,7 +9233,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>535</v>
       </c>
@@ -9077,7 +9250,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>318</v>
       </c>
@@ -9094,7 +9267,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>339</v>
       </c>
@@ -9111,7 +9284,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>536</v>
       </c>
@@ -9128,7 +9301,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>537</v>
       </c>
@@ -9145,7 +9318,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>316</v>
       </c>
@@ -9162,7 +9335,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>576</v>
       </c>
@@ -9179,7 +9352,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>578</v>
       </c>
@@ -9196,7 +9369,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>509</v>
       </c>
@@ -9213,7 +9386,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>217</v>
       </c>
@@ -9230,7 +9403,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>439</v>
       </c>
@@ -9247,7 +9420,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>556</v>
       </c>
@@ -9264,7 +9437,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>154</v>
       </c>
@@ -9281,7 +9454,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>276</v>
       </c>
@@ -9298,7 +9471,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>538</v>
       </c>
@@ -9315,7 +9488,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>456</v>
       </c>
@@ -9332,7 +9505,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>432</v>
       </c>
@@ -9349,7 +9522,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>407</v>
       </c>
@@ -9366,7 +9539,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>360</v>
       </c>
@@ -9383,7 +9556,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>413</v>
       </c>
@@ -9400,7 +9573,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>382</v>
       </c>
@@ -9417,7 +9590,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>356</v>
       </c>
@@ -9434,7 +9607,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>485</v>
       </c>
@@ -9451,7 +9624,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>539</v>
       </c>
@@ -9468,7 +9641,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>540</v>
       </c>
@@ -9485,7 +9658,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>541</v>
       </c>
@@ -9502,7 +9675,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>73</v>
       </c>
@@ -9519,7 +9692,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>457</v>
       </c>
@@ -9536,7 +9709,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>415</v>
       </c>
@@ -9553,7 +9726,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>474</v>
       </c>
@@ -9570,7 +9743,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>435</v>
       </c>
@@ -9587,7 +9760,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>337</v>
       </c>
@@ -9604,7 +9777,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>437</v>
       </c>
@@ -9621,7 +9794,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>481</v>
       </c>
@@ -9638,7 +9811,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>484</v>
       </c>
@@ -9655,7 +9828,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>475</v>
       </c>
@@ -9672,7 +9845,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>323</v>
       </c>
@@ -9689,7 +9862,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>425</v>
       </c>
@@ -9706,7 +9879,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>476</v>
       </c>
@@ -9723,7 +9896,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>370</v>
       </c>
@@ -9740,7 +9913,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>542</v>
       </c>
@@ -9757,7 +9930,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>572</v>
       </c>
@@ -9774,7 +9947,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>543</v>
       </c>
@@ -9791,7 +9964,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>371</v>
       </c>
@@ -9808,7 +9981,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>383</v>
       </c>
@@ -9825,7 +9998,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>305</v>
       </c>
@@ -9842,7 +10015,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>563</v>
       </c>
@@ -9859,7 +10032,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>573</v>
       </c>
@@ -9876,7 +10049,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>394</v>
       </c>
@@ -9893,7 +10066,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>486</v>
       </c>
@@ -9910,7 +10083,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>298</v>
       </c>
@@ -9927,7 +10100,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>458</v>
       </c>
@@ -9944,7 +10117,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>561</v>
       </c>
@@ -9961,7 +10134,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>86</v>
       </c>
@@ -9978,7 +10151,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>327</v>
       </c>
@@ -9995,7 +10168,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>372</v>
       </c>
@@ -10012,7 +10185,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>440</v>
       </c>
@@ -10029,7 +10202,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>441</v>
       </c>
@@ -10046,7 +10219,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>389</v>
       </c>
@@ -10063,7 +10236,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>523</v>
       </c>
@@ -10080,7 +10253,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>384</v>
       </c>
@@ -10097,7 +10270,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>442</v>
       </c>
@@ -10114,7 +10287,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>593</v>
       </c>
@@ -10131,7 +10304,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>348</v>
       </c>
@@ -10148,7 +10321,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>459</v>
       </c>
@@ -10165,7 +10338,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>597</v>
       </c>
@@ -10182,7 +10355,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>140</v>
       </c>
@@ -10199,7 +10372,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>363</v>
       </c>
@@ -10216,7 +10389,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>373</v>
       </c>
@@ -10233,7 +10406,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>302</v>
       </c>
@@ -10250,7 +10423,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>361</v>
       </c>
@@ -10267,7 +10440,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>496</v>
       </c>
@@ -10284,7 +10457,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>325</v>
       </c>
@@ -10301,7 +10474,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>567</v>
       </c>
@@ -10318,7 +10491,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>460</v>
       </c>
@@ -10335,7 +10508,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>319</v>
       </c>
@@ -10352,7 +10525,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>574</v>
       </c>
@@ -10369,7 +10542,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>560</v>
       </c>
@@ -10386,7 +10559,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>506</v>
       </c>
@@ -10403,7 +10576,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>390</v>
       </c>
@@ -10420,7 +10593,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>575</v>
       </c>
@@ -10437,7 +10610,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>357</v>
       </c>
@@ -10454,7 +10627,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>341</v>
       </c>
@@ -10471,7 +10644,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>385</v>
       </c>
@@ -10488,7 +10661,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>416</v>
       </c>
@@ -10505,7 +10678,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>131</v>
       </c>
@@ -10522,7 +10695,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>398</v>
       </c>
@@ -10539,7 +10712,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>405</v>
       </c>
@@ -10556,7 +10729,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>587</v>
       </c>
@@ -10573,7 +10746,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>399</v>
       </c>
@@ -10590,7 +10763,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>426</v>
       </c>
@@ -10607,7 +10780,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>568</v>
       </c>
@@ -10624,7 +10797,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>544</v>
       </c>
@@ -10641,7 +10814,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>391</v>
       </c>
@@ -10658,7 +10831,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>461</v>
       </c>
@@ -10675,7 +10848,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>342</v>
       </c>
@@ -10692,7 +10865,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>374</v>
       </c>
@@ -10709,7 +10882,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>296</v>
       </c>
@@ -10726,7 +10899,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>375</v>
       </c>
@@ -10743,7 +10916,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>380</v>
       </c>
@@ -10760,7 +10933,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>588</v>
       </c>
@@ -10777,7 +10950,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>553</v>
       </c>
@@ -10794,7 +10967,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>462</v>
       </c>
@@ -10811,7 +10984,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>152</v>
       </c>
@@ -10828,7 +11001,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>153</v>
       </c>
@@ -10845,7 +11018,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>24</v>
       </c>
@@ -10862,7 +11035,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>292</v>
       </c>
@@ -10879,7 +11052,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>521</v>
       </c>
@@ -10896,7 +11069,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>545</v>
       </c>
@@ -10913,7 +11086,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>333</v>
       </c>
@@ -10930,7 +11103,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>463</v>
       </c>
@@ -10947,7 +11120,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>546</v>
       </c>
@@ -10964,7 +11137,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>552</v>
       </c>
@@ -10981,7 +11154,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>482</v>
       </c>
@@ -10998,7 +11171,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>497</v>
       </c>
@@ -11015,7 +11188,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>487</v>
       </c>
@@ -11032,7 +11205,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>392</v>
       </c>
@@ -11049,7 +11222,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>328</v>
       </c>
@@ -11066,7 +11239,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>517</v>
       </c>
@@ -11083,7 +11256,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>492</v>
       </c>
@@ -11100,7 +11273,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>477</v>
       </c>
@@ -11117,7 +11290,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>498</v>
       </c>
@@ -11134,7 +11307,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>252</v>
       </c>
@@ -11151,7 +11324,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>581</v>
       </c>
@@ -11168,7 +11341,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>499</v>
       </c>
@@ -11185,7 +11358,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>493</v>
       </c>
@@ -11202,7 +11375,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>494</v>
       </c>
@@ -11219,7 +11392,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>215</v>
       </c>
@@ -11236,7 +11409,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>443</v>
       </c>
@@ -11253,7 +11426,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>259</v>
       </c>
@@ -11270,7 +11443,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>444</v>
       </c>
@@ -11287,7 +11460,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>198</v>
       </c>
@@ -11304,7 +11477,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>344</v>
       </c>
@@ -11321,7 +11494,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>359</v>
       </c>
@@ -11338,7 +11511,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>495</v>
       </c>
@@ -11355,7 +11528,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>376</v>
       </c>
@@ -11372,7 +11545,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>238</v>
       </c>
@@ -11389,7 +11562,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>334</v>
       </c>
@@ -11406,7 +11579,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>590</v>
       </c>
@@ -11423,7 +11596,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>364</v>
       </c>
@@ -11440,7 +11613,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>594</v>
       </c>
@@ -11457,7 +11630,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>408</v>
       </c>
@@ -11474,7 +11647,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>547</v>
       </c>
@@ -11491,7 +11664,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>478</v>
       </c>
@@ -11508,7 +11681,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>548</v>
       </c>
@@ -11525,7 +11698,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>377</v>
       </c>
@@ -11542,7 +11715,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>378</v>
       </c>
@@ -11559,7 +11732,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>417</v>
       </c>
@@ -11576,7 +11749,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>338</v>
       </c>
@@ -11593,7 +11766,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>579</v>
       </c>
@@ -11610,7 +11783,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>400</v>
       </c>
@@ -11627,7 +11800,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>329</v>
       </c>
@@ -11644,7 +11817,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>515</v>
       </c>
@@ -11661,7 +11834,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>500</v>
       </c>
@@ -11678,7 +11851,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>221</v>
       </c>
@@ -11695,7 +11868,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>409</v>
       </c>
@@ -11712,7 +11885,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>464</v>
       </c>
@@ -11729,7 +11902,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>410</v>
       </c>
@@ -11746,7 +11919,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>324</v>
       </c>
@@ -11763,7 +11936,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>349</v>
       </c>
@@ -11780,7 +11953,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>558</v>
       </c>
@@ -11797,7 +11970,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>281</v>
       </c>
@@ -11814,7 +11987,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>401</v>
       </c>
@@ -11831,7 +12004,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>246</v>
       </c>
@@ -11848,7 +12021,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>263</v>
       </c>
@@ -11865,7 +12038,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>354</v>
       </c>
@@ -11882,7 +12055,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>386</v>
       </c>
@@ -11899,7 +12072,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>518</v>
       </c>
@@ -11916,7 +12089,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>249</v>
       </c>
@@ -11933,7 +12106,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>418</v>
       </c>
@@ -11950,7 +12123,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>205</v>
       </c>
@@ -11967,7 +12140,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>554</v>
       </c>
@@ -11984,7 +12157,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>501</v>
       </c>
@@ -12001,7 +12174,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>549</v>
       </c>
@@ -12018,7 +12191,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>598</v>
       </c>
@@ -12035,7 +12208,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>502</v>
       </c>
@@ -12052,7 +12225,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>564</v>
       </c>
@@ -12069,7 +12242,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>303</v>
       </c>
@@ -12086,7 +12259,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>427</v>
       </c>
@@ -12103,7 +12276,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>402</v>
       </c>
@@ -12120,7 +12293,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>550</v>
       </c>
@@ -12137,7 +12310,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>445</v>
       </c>
@@ -12154,7 +12327,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>379</v>
       </c>
@@ -12171,7 +12344,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>446</v>
       </c>
@@ -12188,7 +12361,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>393</v>
       </c>
@@ -12205,7 +12378,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>428</v>
       </c>
@@ -12222,7 +12395,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>358</v>
       </c>
@@ -12239,7 +12412,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>526</v>
       </c>
@@ -12256,7 +12429,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>353</v>
       </c>
@@ -12273,7 +12446,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>299</v>
       </c>
@@ -12290,7 +12463,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>565</v>
       </c>
@@ -12307,7 +12480,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>395</v>
       </c>
@@ -12324,7 +12497,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>429</v>
       </c>
@@ -12341,7 +12514,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>300</v>
       </c>
@@ -12358,7 +12531,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>184</v>
       </c>
@@ -12375,7 +12548,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>411</v>
       </c>
@@ -12392,7 +12565,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>465</v>
       </c>
@@ -12409,7 +12582,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>309</v>
       </c>
@@ -12426,7 +12599,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>557</v>
       </c>
@@ -12443,7 +12616,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>522</v>
       </c>
@@ -12460,7 +12633,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>436</v>
       </c>
@@ -12477,7 +12650,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>304</v>
       </c>
@@ -12494,7 +12667,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>466</v>
       </c>
@@ -12511,7 +12684,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>430</v>
       </c>
@@ -12528,7 +12701,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>524</v>
       </c>
@@ -12545,7 +12718,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>514</v>
       </c>
@@ -12562,7 +12735,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>479</v>
       </c>
@@ -12579,7 +12752,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>595</v>
       </c>
@@ -12596,7 +12769,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>19</v>
       </c>
@@ -12613,7 +12786,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>570</v>
       </c>
@@ -12630,7 +12803,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>311</v>
       </c>
@@ -12647,7 +12820,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>330</v>
       </c>
@@ -12664,7 +12837,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>412</v>
       </c>
@@ -12681,7 +12854,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>480</v>
       </c>
@@ -12698,7 +12871,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>320</v>
       </c>
@@ -12715,7 +12888,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>467</v>
       </c>
@@ -12732,7 +12905,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>419</v>
       </c>
@@ -12749,7 +12922,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>362</v>
       </c>
@@ -12766,7 +12939,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>468</v>
       </c>
@@ -12783,7 +12956,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>335</v>
       </c>
@@ -12800,7 +12973,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>551</v>
       </c>
@@ -12817,7 +12990,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>56</v>
       </c>
@@ -12834,7 +13007,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>447</v>
       </c>
@@ -12851,7 +13024,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>589</v>
       </c>
@@ -12868,7 +13041,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>343</v>
       </c>

</xml_diff>